<commit_message>
major: added meshing chapter - todo: maybe transform excel graph to tikz?
</commit_message>
<xml_diff>
--- a/simulations/Grid_convergence/GCI_Study.xlsx
+++ b/simulations/Grid_convergence/GCI_Study.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f6ef27e316a124d/MCI/Semester_3/FLUID_CFD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\Documents\MCI\optimization-of-a-heater---CFD-report\simulations\Grid_convergence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{84E1B584-0795-4EEA-84B0-30DD14AD3A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78A77271-2AF5-4F1B-8E89-4A3EDF0AF956}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE975F94-A73C-4F2F-9480-033F3B75C6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorlage" sheetId="1" r:id="rId1"/>
@@ -1505,8 +1505,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Norm. Grid Spacing / -</a:t>
+                  <a:t>Mesh</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> size [mm]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1636,8 +1641,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>|v_MAX| @ extract / (m/s)</a:t>
+                  <a:t>average</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> temperature 25 mm before outlet</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -5824,19 +5834,19 @@
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5850,12 +5860,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>4</v>
@@ -5867,7 +5877,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -5881,7 +5891,7 @@
         <v>0.14469000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -5895,7 +5905,7 @@
         <v>0.14688000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -5909,12 +5919,12 @@
         <v>0.14752000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -5922,7 +5932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -5931,12 +5941,12 @@
         <v>1.7747870596011681</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8">
@@ -5947,7 +5957,7 @@
         <v>0.14752000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -5959,12 +5969,12 @@
         <v>0.14778425806451614</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -5972,7 +5982,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>18</v>
       </c>
@@ -5984,7 +5994,7 @@
         <v>7.695551338815128E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>19</v>
       </c>
@@ -5996,24 +6006,24 @@
         <v>2.2391715065425968E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D34" s="10">
         <f>D32</f>
         <v>7.695551338815128E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D35" s="10">
         <f>D33</f>
         <v>2.2391715065425968E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>23</v>
       </c>
@@ -6037,19 +6047,19 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -6063,12 +6073,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>4</v>
@@ -6080,7 +6090,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -6094,7 +6104,7 @@
         <v>305.52</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -6108,7 +6118,7 @@
         <v>303.52</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -6122,12 +6132,12 @@
         <v>303.24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -6135,7 +6145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -6144,12 +6154,12 @@
         <v>2.8365012677172614</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8">
@@ -6160,7 +6170,7 @@
         <v>303.24</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -6172,12 +6182,12 @@
         <v>303.19441860465116</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -6185,7 +6195,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>18</v>
       </c>
@@ -6197,7 +6207,7 @@
         <v>1.3408564318199802E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>19</v>
       </c>
@@ -6209,24 +6219,24 @@
         <v>1.8789323369619609E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D34" s="10">
         <f>D32</f>
         <v>1.3408564318199802E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D35" s="10">
         <f>D33</f>
         <v>1.8789323369619609E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>23</v>
       </c>
@@ -6246,23 +6256,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34585E80-F101-4E63-9099-C0A13B56FCA8}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -6276,12 +6286,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>4</v>
@@ -6293,7 +6303,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -6307,7 +6317,7 @@
         <v>305.62</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -6321,7 +6331,7 @@
         <v>304.95999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -6335,12 +6345,12 @@
         <v>304.69</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -6348,7 +6358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -6357,12 +6367,12 @@
         <v>1.2895066171951368</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8">
@@ -6373,7 +6383,7 @@
         <v>304.69</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -6385,12 +6395,12 @@
         <v>304.50307692307695</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -6398,7 +6408,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>18</v>
       </c>
@@ -6410,7 +6420,7 @@
         <v>1.8728811849218457E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>19</v>
       </c>
@@ -6422,24 +6432,24 @@
         <v>7.6685761316022444E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D34" s="10">
         <f>D32</f>
         <v>1.8728811849218457E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D35" s="10">
         <f>D33</f>
         <v>7.6685761316022444E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>23</v>
       </c>
@@ -6459,23 +6469,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69053333-2CFB-47FC-BD8B-B2157D00B61E}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -6489,12 +6499,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>4</v>
@@ -6506,7 +6516,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -6520,7 +6530,7 @@
         <v>304.95999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -6534,7 +6544,7 @@
         <v>304.69</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -6548,12 +6558,12 @@
         <v>304.66000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -6561,7 +6571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -6570,12 +6580,12 @@
         <v>3.1699250014435276</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8">
@@ -6586,7 +6596,7 @@
         <v>304.66000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -6598,12 +6608,12 @@
         <v>304.65625000000006</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -6611,7 +6621,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>18</v>
       </c>
@@ -6623,7 +6633,7 @@
         <v>1.3846040237604511E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>19</v>
       </c>
@@ -6635,24 +6645,24 @@
         <v>1.538600407008237E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D34" s="10">
         <f>D32</f>
         <v>1.3846040237604511E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D35" s="10">
         <f>D33</f>
         <v>1.538600407008237E-5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>23</v>
       </c>

</xml_diff>